<commit_message>
enriquecimento e filtro de targets e terms
</commit_message>
<xml_diff>
--- a/Deseq2/SRP151491 - M tuberculosis/results/PCA_Uninfected_vs_Infected.xlsx
+++ b/Deseq2/SRP151491 - M tuberculosis/results/PCA_Uninfected_vs_Infected.xlsx
@@ -437,10 +437,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-19.1105264303336</v>
+        <v>-19.2308319290313</v>
       </c>
       <c r="B2" t="n">
-        <v>-7.06575660390109</v>
+        <v>-6.97169899366997</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -454,10 +454,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-23.9088634263519</v>
+        <v>-23.9802852812849</v>
       </c>
       <c r="B3" t="n">
-        <v>-7.95003409638865</v>
+        <v>-7.7982463176201</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -471,10 +471,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-16.9431962262717</v>
+        <v>-16.960506082904</v>
       </c>
       <c r="B4" t="n">
-        <v>-5.32895399274582</v>
+        <v>-5.21503806213296</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -488,10 +488,10 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-6.06549750917738</v>
+        <v>-6.0557950345974</v>
       </c>
       <c r="B5" t="n">
-        <v>8.57790491722823</v>
+        <v>8.66878944083269</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -505,10 +505,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-8.35913825840571</v>
+        <v>-8.3173126196345</v>
       </c>
       <c r="B6" t="n">
-        <v>7.6240831355463</v>
+        <v>7.72200995182726</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -522,10 +522,10 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-11.757628477918</v>
+        <v>-11.7390376770988</v>
       </c>
       <c r="B7" t="n">
-        <v>6.49185829885045</v>
+        <v>6.55014202270683</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -539,10 +539,10 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>-30.8601946566561</v>
+        <v>-30.9038875155909</v>
       </c>
       <c r="B8" t="n">
-        <v>-5.89774592613417</v>
+        <v>-5.67362107160279</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -556,10 +556,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>-29.6650838065069</v>
+        <v>-29.7553818137461</v>
       </c>
       <c r="B9" t="n">
-        <v>-5.74227647765456</v>
+        <v>-5.54597823818038</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -573,10 +573,10 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>-31.6410371149056</v>
+        <v>-31.7424471672916</v>
       </c>
       <c r="B10" t="n">
-        <v>-4.35272141710977</v>
+        <v>-4.05570839629435</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -590,10 +590,10 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>26.3718638886718</v>
+        <v>26.0426481467496</v>
       </c>
       <c r="B11" t="n">
-        <v>-31.4381342669928</v>
+        <v>-31.5358823004391</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -607,10 +607,10 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>25.5870878896587</v>
+        <v>25.2837058303201</v>
       </c>
       <c r="B12" t="n">
-        <v>-31.1858483691458</v>
+        <v>-31.278645391384</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -624,10 +624,10 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>25.7473328138684</v>
+        <v>25.4608257560563</v>
       </c>
       <c r="B13" t="n">
-        <v>-29.7367463964854</v>
+        <v>-29.8284757647492</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -641,10 +641,10 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13.7765968841705</v>
+        <v>14.0268080440438</v>
       </c>
       <c r="B14" t="n">
-        <v>24.2814271555979</v>
+        <v>24.1892809280537</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -658,10 +658,10 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>15.1960322016727</v>
+        <v>15.4484645424469</v>
       </c>
       <c r="B15" t="n">
-        <v>24.9057253944775</v>
+        <v>24.7659992746942</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
@@ -675,10 +675,10 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14.4704818421971</v>
+        <v>14.7996743493779</v>
       </c>
       <c r="B16" t="n">
-        <v>25.4757943498909</v>
+        <v>25.3144793526506</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -692,10 +692,10 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>19.084292659248</v>
+        <v>19.2306529098194</v>
       </c>
       <c r="B17" t="n">
-        <v>10.2577276535694</v>
+        <v>10.0243896118943</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -709,10 +709,10 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>18.4254013408354</v>
+        <v>18.5855206174471</v>
       </c>
       <c r="B18" t="n">
-        <v>10.1363126574142</v>
+        <v>9.92749469351463</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
@@ -726,10 +726,10 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>19.6520763862042</v>
+        <v>19.8071849249185</v>
       </c>
       <c r="B19" t="n">
-        <v>10.9473839839831</v>
+        <v>10.7407092598987</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>

</xml_diff>